<commit_message>
push - bug fix + feedback update
</commit_message>
<xml_diff>
--- a/outputs/feedback_full.xlsx
+++ b/outputs/feedback_full.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,11 +477,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>154950</v>
+        <v>156244</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mart Minas, 12/08/2024</t>
+          <t>FBMDS, 29/07/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -501,27 +501,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
+          <t>Planejamento foi reprovado</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-08-12</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>FBMDS</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>154950</v>
+        <v>156244</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mart Minas, 12/08/2024</t>
+          <t>FBMDS, 29/07/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -541,27 +541,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cliente solicitou ajustes ou refação</t>
+          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-08-12</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>FBMDS</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>153488</v>
+        <v>156243</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mart Minas, 07/08/2024</t>
+          <t>Litero, 05/08/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -581,27 +581,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Cliente solicitou ajustes ou refação</t>
+          <t>Cliente pediu proposta</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-05</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>Litero</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>153488</v>
+        <v>156243</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mart Minas, 07/08/2024</t>
+          <t>Litero, 05/08/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -621,27 +621,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Entregas feitas conforme planejado</t>
+          <t>Feedback positivo</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-05</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>Litero</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>149896</v>
+        <v>154950</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mart Minas, 15/07/2024</t>
+          <t>Mart Minas, 12/08/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Metas não atingidas</t>
+          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -677,11 +677,11 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>149896</v>
+        <v>154950</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mart Minas, 15/07/2024</t>
+          <t>Mart Minas, 12/08/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -701,12 +701,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Feedback positivo</t>
+          <t>Cliente solicitou ajustes ou refação</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -717,11 +717,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>148735</v>
+        <v>153488</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15/07/2024</t>
+          <t>Mart Minas, 07/08/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -739,25 +739,29 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Cliente solicitou ajustes ou refação</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-08-07</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Iteris</t>
+          <t>Mart Minas</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>148734</v>
+        <v>153488</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>Mart Minas, 07/08/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -777,27 +781,27 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Cliente pediu proposta</t>
+          <t>Entregas feitas conforme planejado</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-08-07</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Evera</t>
+          <t>Mart Minas</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>148734</v>
+        <v>149896</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24/06/2024</t>
+          <t>Mart Minas, 15/07/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -822,22 +826,22 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-07-15</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Evera</t>
+          <t>Mart Minas</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>148717</v>
+        <v>149896</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Positivo - 20/07</t>
+          <t>Mart Minas, 15/07/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -855,217 +859,21 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>145864</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ITA, 14/06/2024</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Feedback negativo</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2024-06-14</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>145864</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ITA, 14/06/2024</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2024-06-14</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>145864</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ITA, 14/06/2024</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Metas não atingidas</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2024-06-14</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>145783</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Positivo, 05/07/2024</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Cliente pediu proposta</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2024-07-05</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>145783</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Positivo, 05/07/2024</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Feedback positivo</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2024-07-05</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>144154</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Teste Healthscore</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2024-07-15</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
push - rename + update
</commit_message>
<xml_diff>
--- a/outputs/feedback_full.xlsx
+++ b/outputs/feedback_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,11 +477,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>156244</v>
+        <v>157844</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FBMDS, 29/07/2024</t>
+          <t>Mart Minas, 19/08/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -501,27 +501,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Planejamento foi reprovado</t>
+          <t>Cliente solicitou ajustes ou refação</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-19</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FBMDS</t>
+          <t>Mart Minas</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>156244</v>
+        <v>157844</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FBMDS, 29/07/2024</t>
+          <t>Mart Minas, 19/08/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -541,27 +541,27 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
+          <t>Entregas feitas conforme planejado</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-19</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>FBMDS</t>
+          <t>Mart Minas</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>156243</v>
+        <v>157821</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Litero, 05/08/2024</t>
+          <t>Cocamar, 15/07/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -586,22 +586,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-08-05</t>
+          <t>2024-07-15</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Litero</t>
+          <t>Cocamar</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>156243</v>
+        <v>157821</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Litero, 05/08/2024</t>
+          <t>Cocamar, 15/07/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -621,27 +621,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Feedback positivo</t>
+          <t>Resolveu problema</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-08-05</t>
+          <t>2024-07-15</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Litero</t>
+          <t>Cocamar</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>154950</v>
+        <v>156244</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mart Minas, 12/08/2024</t>
+          <t>FBMDS, 29/07/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,27 +661,27 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
+          <t>Planejamento foi reprovado</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-08-12</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>FBMDS</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>154950</v>
+        <v>156244</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mart Minas, 12/08/2024</t>
+          <t>FBMDS, 29/07/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -701,27 +701,27 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Cliente solicitou ajustes ou refação</t>
+          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-08-12</t>
+          <t>2024-07-29</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>FBMDS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>153488</v>
+        <v>156243</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mart Minas, 07/08/2024</t>
+          <t>Litero, 05/08/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -741,27 +741,27 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Cliente solicitou ajustes ou refação</t>
+          <t>Cliente pediu proposta</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-05</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>Litero</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>153488</v>
+        <v>156243</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mart Minas, 07/08/2024</t>
+          <t>Litero, 05/08/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -781,27 +781,27 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Entregas feitas conforme planejado</t>
+          <t>Feedback positivo</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2024-08-07</t>
+          <t>2024-08-05</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Mart Minas</t>
+          <t>Litero</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>149896</v>
+        <v>154950</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mart Minas, 15/07/2024</t>
+          <t>Mart Minas, 12/08/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -821,12 +821,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Metas não atingidas</t>
+          <t>Houve atraso nas entregas, isso prejudicou os clientes</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -837,39 +837,199 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>154950</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mart Minas, 12/08/2024</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Cliente solicitou ajustes ou refação</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2024-08-12</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>153488</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mart Minas, 07/08/2024</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Cliente solicitou ajustes ou refação</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2024-08-07</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>153488</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mart Minas, 07/08/2024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Entregas feitas conforme planejado</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2024-08-07</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>149896</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Mart Minas, 15/07/2024</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>backlog</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Acompanhamento de clientes</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Metas não atingidas</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2024-07-15</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Mart Minas</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>149896</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mart Minas, 15/07/2024</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>backlog</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Acompanhamento de clientes</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>Feedback positivo</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>2024-07-15</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Mart Minas</t>
         </is>

</xml_diff>